<commit_message>
Created testing file for EMA smoothing factor
</commit_message>
<xml_diff>
--- a/Testing RSSI average methods.xlsx
+++ b/Testing RSSI average methods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joryl\Dissertation\dissertation_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{172944F3-16F5-47E4-B5F4-E23760E7945D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69CE79EA-2201-42D9-AB93-529F3FC6891B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="6" xr2:uid="{7F11D34D-8D55-4517-9872-D5C4F32D54AF}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>MEAN</t>
   </si>
@@ -128,9 +128,6 @@
   <si>
     <t>Column4</t>
   </si>
-  <si>
-    <t xml:space="preserve">*Chosen as best compromise between stability and responsiveness </t>
-  </si>
 </sst>
 </file>
 
@@ -173,17 +170,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2466,17 +2457,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{881E5496-3077-4AF9-975C-04A27FA68ED7}">
-  <dimension ref="A2:N66"/>
+  <dimension ref="A2:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.109375" customWidth="1"/>
     <col min="7" max="7" width="17.6640625" customWidth="1"/>
-    <col min="9" max="9" width="35.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="35.33203125" customWidth="1"/>
     <col min="10" max="10" width="22.88671875" customWidth="1"/>
     <col min="11" max="11" width="23" customWidth="1"/>
     <col min="12" max="13" width="22.33203125" customWidth="1"/>
@@ -2501,42 +2492,39 @@
       <c r="G4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="N4" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="5" spans="1:14" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="M5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="N5" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2553,22 +2541,22 @@
       <c r="G6">
         <v>-44.7</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6">
         <v>-52</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6">
         <v>-46</v>
       </c>
       <c r="K6">
         <v>-46</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6">
         <v>-52</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6">
         <v>-58</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6">
         <v>-60</v>
       </c>
     </row>
@@ -2585,22 +2573,22 @@
       <c r="G7">
         <v>-45.3</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7">
         <v>-52</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7">
         <v>-46</v>
       </c>
       <c r="K7">
         <v>-46</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7">
         <v>-52.1</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7">
         <v>-57.9</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7">
         <v>-59.9</v>
       </c>
     </row>
@@ -2617,22 +2605,22 @@
       <c r="G8">
         <v>-41.3</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8">
         <v>-50.4</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8">
         <v>-45.6</v>
       </c>
       <c r="K8">
         <v>-45.6</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8">
         <v>-52.7</v>
       </c>
-      <c r="M8" s="4">
+      <c r="M8">
         <v>-57.8</v>
       </c>
-      <c r="N8" s="4">
+      <c r="N8">
         <v>-59.4</v>
       </c>
     </row>
@@ -2649,22 +2637,22 @@
       <c r="G9">
         <v>-42</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9">
         <v>-49.1</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9">
         <v>-45.2</v>
       </c>
       <c r="K9">
         <v>-45.2</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9">
         <v>-52.8</v>
       </c>
-      <c r="M9" s="4">
+      <c r="M9">
         <v>-57.6</v>
       </c>
-      <c r="N9" s="4">
+      <c r="N9">
         <v>-59.8</v>
       </c>
     </row>
@@ -2681,22 +2669,22 @@
       <c r="G10">
         <v>-40</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10">
         <v>-49.3</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10">
         <v>-44.3</v>
       </c>
       <c r="K10">
         <v>-44.3</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10">
         <v>-53.1</v>
       </c>
-      <c r="M10" s="4">
+      <c r="M10">
         <v>-57.3</v>
       </c>
-      <c r="N10" s="4">
+      <c r="N10">
         <v>-59.9</v>
       </c>
     </row>
@@ -2710,22 +2698,22 @@
       <c r="E11">
         <v>-40</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11">
         <v>-49.4</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11">
         <v>-43.5</v>
       </c>
       <c r="K11">
         <v>-43.5</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11">
         <v>-53.4</v>
       </c>
-      <c r="M11" s="4">
+      <c r="M11">
         <v>-57.3</v>
       </c>
-      <c r="N11" s="4">
+      <c r="N11">
         <v>-59.5</v>
       </c>
     </row>
@@ -2736,22 +2724,22 @@
       <c r="C12">
         <v>-38.4</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12">
         <v>-49.5</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12">
         <v>-44.7</v>
       </c>
       <c r="K12">
         <v>-44.7</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12">
         <v>-53.7</v>
       </c>
-      <c r="M12" s="4">
+      <c r="M12">
         <v>-57.2</v>
       </c>
-      <c r="N12" s="4">
+      <c r="N12">
         <v>-59.3</v>
       </c>
     </row>
@@ -2762,22 +2750,22 @@
       <c r="C13">
         <v>-38.4</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13">
         <v>-48.4</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13">
         <v>-44.3</v>
       </c>
       <c r="K13">
         <v>-44.3</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13">
         <v>-53.7</v>
       </c>
-      <c r="M13" s="4">
+      <c r="M13">
         <v>-56.9</v>
       </c>
-      <c r="N13" s="4">
+      <c r="N13">
         <v>-59</v>
       </c>
     </row>
@@ -2788,22 +2776,22 @@
       <c r="C14">
         <v>-41.2</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14">
         <v>-48.4</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J14">
         <v>-43.8</v>
       </c>
       <c r="K14">
         <v>-43.8</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14">
         <v>-53.7</v>
       </c>
-      <c r="M14" s="4">
+      <c r="M14">
         <v>-56.7</v>
       </c>
-      <c r="N14" s="4">
+      <c r="N14">
         <v>-58.8</v>
       </c>
     </row>
@@ -2811,639 +2799,544 @@
       <c r="A15">
         <v>-40</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15">
         <v>-47.5</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J15">
         <v>-43.5</v>
       </c>
       <c r="K15">
         <v>-43.5</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15">
         <v>-53.7</v>
       </c>
-      <c r="M15" s="4">
+      <c r="M15">
         <v>-56.5</v>
       </c>
-      <c r="N15" s="4">
+      <c r="N15">
         <v>-58.6</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="I16" s="4">
+      <c r="I16">
         <v>-46.8</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J16">
         <v>-42.7</v>
       </c>
       <c r="K16">
         <v>-42.7</v>
       </c>
-      <c r="L16" s="4">
+      <c r="L16">
         <v>-53.7</v>
       </c>
-      <c r="M16" s="4">
+      <c r="M16">
         <v>-56.4</v>
       </c>
-      <c r="N16" s="4">
+      <c r="N16">
         <v>-58.4</v>
       </c>
     </row>
     <row r="17" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I17" s="4">
+      <c r="I17">
         <v>-46.6</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J17">
         <v>-42.2</v>
       </c>
       <c r="K17">
         <v>-42.2</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17">
         <v>-53.9</v>
       </c>
-      <c r="M17" s="4">
+      <c r="M17">
         <v>-56.3</v>
       </c>
-      <c r="N17" s="4">
+      <c r="N17">
         <v>-58.3</v>
       </c>
     </row>
     <row r="18" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I18" s="4">
+      <c r="I18">
         <v>-46.5</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J18">
         <v>-41.6</v>
       </c>
       <c r="K18">
         <v>-41.6</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L18">
         <v>-54.2</v>
       </c>
-      <c r="M18" s="4">
+      <c r="M18">
         <v>-56.1</v>
       </c>
-      <c r="N18" s="4">
+      <c r="N18">
         <v>-58</v>
       </c>
     </row>
     <row r="19" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I19" s="4">
+      <c r="I19">
         <v>-47.6</v>
       </c>
-      <c r="J19" s="4">
+      <c r="J19">
         <v>-41.1</v>
       </c>
       <c r="K19">
         <v>-41.1</v>
       </c>
-      <c r="L19" s="4">
+      <c r="L19">
         <v>-54.5</v>
       </c>
-      <c r="M19" s="4">
+      <c r="M19">
         <v>-55.9</v>
       </c>
-      <c r="N19" s="4">
+      <c r="N19">
         <v>-57.8</v>
       </c>
     </row>
     <row r="20" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I20" s="4">
+      <c r="I20">
         <v>-48.5</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J20">
         <v>-40.5</v>
       </c>
       <c r="K20">
         <v>-40.5</v>
       </c>
-      <c r="L20" s="4">
+      <c r="L20">
         <v>-54.8</v>
       </c>
-      <c r="M20" s="4">
+      <c r="M20">
         <v>-55.7</v>
       </c>
-      <c r="N20" s="4">
+      <c r="N20">
         <v>-57.6</v>
       </c>
     </row>
     <row r="21" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I21" s="4">
+      <c r="I21">
         <v>-49.2</v>
       </c>
-      <c r="J21" s="4">
+      <c r="J21">
         <v>-40.1</v>
       </c>
       <c r="K21">
         <v>-40.1</v>
       </c>
-      <c r="L21" s="4">
+      <c r="L21">
         <v>-54.8</v>
       </c>
-      <c r="M21" s="4">
+      <c r="M21">
         <v>-55.5</v>
       </c>
-      <c r="N21" s="4">
+      <c r="N21">
         <v>-57.3</v>
       </c>
     </row>
     <row r="22" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I22" s="4">
+      <c r="I22">
         <v>-49.7</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J22">
         <v>-40.1</v>
       </c>
       <c r="K22">
         <v>-40.1</v>
       </c>
-      <c r="L22" s="4">
+      <c r="L22">
         <v>-54.7</v>
       </c>
-      <c r="M22" s="4">
+      <c r="M22">
         <v>-55.3</v>
       </c>
-      <c r="N22" s="4">
+      <c r="N22">
         <v>-57.1</v>
       </c>
     </row>
     <row r="23" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I23" s="4">
+      <c r="I23">
         <v>-50.2</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J23">
         <v>-40.1</v>
       </c>
       <c r="K23">
         <v>-40.1</v>
       </c>
-      <c r="L23" s="4">
+      <c r="L23">
         <v>-54.7</v>
       </c>
-      <c r="M23" s="4">
+      <c r="M23">
         <v>-55.3</v>
       </c>
-      <c r="N23" s="4">
+      <c r="N23">
         <v>-56.9</v>
       </c>
     </row>
     <row r="24" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I24" s="4">
+      <c r="I24">
         <v>-49</v>
       </c>
-      <c r="J24" s="4">
+      <c r="J24">
         <v>-39.700000000000003</v>
       </c>
       <c r="K24">
         <v>-39.700000000000003</v>
       </c>
-      <c r="L24" s="4">
+      <c r="L24">
         <v>-54.6</v>
       </c>
-      <c r="M24" s="4">
+      <c r="M24">
         <v>-55.1</v>
       </c>
-      <c r="N24" s="4">
+      <c r="N24">
         <v>-56.7</v>
       </c>
     </row>
     <row r="25" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I25" s="4">
+      <c r="I25">
         <v>-48.4</v>
       </c>
-      <c r="J25" s="4">
+      <c r="J25">
         <v>-39.299999999999997</v>
       </c>
       <c r="K25">
         <v>-39.299999999999997</v>
       </c>
-      <c r="L25" s="4">
+      <c r="L25">
         <v>-54.6</v>
       </c>
-      <c r="M25" s="4">
+      <c r="M25">
         <v>-55</v>
       </c>
-      <c r="N25" s="4">
+      <c r="N25">
         <v>-56.5</v>
       </c>
     </row>
     <row r="26" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I26" s="4">
+      <c r="I26">
         <v>-47.9</v>
       </c>
-      <c r="J26" s="4">
+      <c r="J26">
         <v>-39.4</v>
       </c>
       <c r="K26">
         <v>-39.4</v>
       </c>
-      <c r="L26" s="4">
+      <c r="L26">
         <v>-56</v>
       </c>
-      <c r="M26" s="4">
+      <c r="M26">
         <v>-54.7</v>
       </c>
-      <c r="N26" s="4">
+      <c r="N26">
         <v>-56.3</v>
       </c>
     </row>
     <row r="27" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I27" s="4">
+      <c r="I27">
         <v>-47.1</v>
       </c>
-      <c r="J27" s="4">
+      <c r="J27">
         <v>-39.4</v>
       </c>
       <c r="K27">
         <v>-39.4</v>
       </c>
-      <c r="L27" s="4">
+      <c r="L27">
         <v>-56</v>
       </c>
-      <c r="M27" s="4">
+      <c r="M27">
         <v>-54.5</v>
       </c>
-      <c r="N27" s="4">
+      <c r="N27">
         <v>-56.8</v>
       </c>
     </row>
     <row r="28" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I28" s="4">
+      <c r="I28">
         <v>-46.5</v>
       </c>
-      <c r="J28" s="4">
+      <c r="J28">
         <v>-39.299999999999997</v>
       </c>
       <c r="K28">
         <v>-39.299999999999997</v>
       </c>
-      <c r="L28" s="4">
+      <c r="L28">
         <v>-56</v>
       </c>
-      <c r="M28" s="4">
+      <c r="M28">
         <v>-54.3</v>
       </c>
-      <c r="N28" s="4">
+      <c r="N28">
         <v>-57.2</v>
       </c>
     </row>
     <row r="29" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I29" s="4">
+      <c r="I29">
         <v>-46.4</v>
       </c>
-      <c r="J29" s="4">
+      <c r="J29">
         <v>-39.200000000000003</v>
       </c>
       <c r="K29">
         <v>-39.200000000000003</v>
       </c>
-      <c r="L29" s="4">
+      <c r="L29">
         <v>-56.1</v>
       </c>
-      <c r="M29" s="4">
+      <c r="M29">
         <v>-54.2</v>
       </c>
-      <c r="N29" s="4">
+      <c r="N29">
         <v>-57.3</v>
       </c>
     </row>
     <row r="30" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I30" s="4">
+      <c r="I30">
         <v>-46.3</v>
       </c>
-      <c r="J30" s="4">
+      <c r="J30">
         <v>-39.200000000000003</v>
       </c>
       <c r="K30">
         <v>-40</v>
       </c>
-      <c r="L30" s="4">
+      <c r="L30">
         <v>-56.1</v>
       </c>
-      <c r="M30" s="4">
+      <c r="M30">
         <v>-54.1</v>
       </c>
-      <c r="N30" s="4">
+      <c r="N30">
         <v>-57.2</v>
       </c>
     </row>
     <row r="31" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I31" s="4">
+      <c r="I31">
         <v>-46.3</v>
       </c>
-      <c r="J31" s="4">
+      <c r="J31">
         <v>-39.299999999999997</v>
       </c>
       <c r="K31">
         <v>-40</v>
       </c>
-      <c r="L31" s="4">
+      <c r="L31">
         <v>-55.9</v>
       </c>
-      <c r="M31" s="4">
+      <c r="M31">
         <v>-53.9</v>
       </c>
-      <c r="N31" s="4">
+      <c r="N31">
         <v>-57.2</v>
       </c>
     </row>
     <row r="32" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I32" s="4">
+      <c r="I32">
         <v>-47.4</v>
       </c>
-      <c r="J32" s="4">
+      <c r="J32">
         <v>-39.4</v>
       </c>
       <c r="K32">
         <v>-40.9</v>
       </c>
-      <c r="L32" s="4">
+      <c r="L32">
         <v>-55.6</v>
       </c>
-      <c r="M32" s="4">
+      <c r="M32">
         <v>-54.1</v>
       </c>
-      <c r="N32" s="4">
+      <c r="N32">
         <v>-57.1</v>
       </c>
     </row>
     <row r="33" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I33" s="4">
+      <c r="I33">
         <v>-48.3</v>
       </c>
-      <c r="J33" s="4">
+      <c r="J33">
         <v>-39.4</v>
       </c>
       <c r="K33">
         <v>-41.7</v>
       </c>
-      <c r="L33" s="4">
+      <c r="L33">
         <v>-55.4</v>
       </c>
-      <c r="M33" s="4">
+      <c r="M33">
         <v>-54.3</v>
       </c>
-      <c r="N33" s="4">
+      <c r="N33">
         <v>-56.9</v>
       </c>
     </row>
     <row r="34" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I34" s="4">
+      <c r="I34">
         <v>-49.1</v>
       </c>
-      <c r="J34" s="4">
+      <c r="J34">
         <v>-39.299999999999997</v>
       </c>
       <c r="K34">
         <v>-42.6</v>
       </c>
-      <c r="L34" s="4">
+      <c r="L34">
         <v>-55.3</v>
       </c>
-      <c r="M34" s="4">
+      <c r="M34">
         <v>-54.5</v>
       </c>
-      <c r="N34" s="4">
+      <c r="N34">
         <v>-56.7</v>
       </c>
     </row>
     <row r="35" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I35" s="4">
+      <c r="I35">
         <v>-49.6</v>
       </c>
-      <c r="J35" s="4">
+      <c r="J35">
         <v>-39.200000000000003</v>
       </c>
       <c r="K35">
         <v>-43.4</v>
       </c>
-      <c r="L35" s="4">
+      <c r="L35">
         <v>-55.1</v>
       </c>
-      <c r="M35" s="4">
+      <c r="M35">
         <v>-54.6</v>
       </c>
-      <c r="N35" s="4">
+      <c r="N35">
         <v>-58.3</v>
       </c>
     </row>
     <row r="36" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I36" s="4">
+      <c r="I36">
         <v>-48.5</v>
       </c>
-      <c r="J36" s="4">
+      <c r="J36">
         <v>-38.9</v>
       </c>
       <c r="K36">
         <v>-43.2</v>
       </c>
-      <c r="L36" s="4">
+      <c r="L36">
         <v>-54.9</v>
       </c>
-      <c r="M36" s="4">
+      <c r="M36">
         <v>-54.8</v>
       </c>
-      <c r="N36" s="4">
+      <c r="N36">
         <v>-58</v>
       </c>
     </row>
     <row r="37" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I37" s="4">
+      <c r="I37">
         <v>-47.6</v>
       </c>
-      <c r="J37" s="4">
+      <c r="J37">
         <v>-38.799999999999997</v>
       </c>
       <c r="K37">
         <v>-43</v>
       </c>
-      <c r="L37" s="4">
+      <c r="L37">
         <v>-55.2</v>
       </c>
-      <c r="M37" s="4">
+      <c r="M37">
         <v>-55</v>
       </c>
-      <c r="N37" s="4">
+      <c r="N37">
         <v>-57.8</v>
       </c>
     </row>
     <row r="38" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I38" s="4">
+      <c r="I38">
         <v>-46.9</v>
       </c>
-      <c r="J38" s="4">
+      <c r="J38">
         <v>-38.5</v>
       </c>
       <c r="K38">
         <v>-43.2</v>
       </c>
-      <c r="L38" s="4">
+      <c r="L38">
         <v>-55</v>
       </c>
-      <c r="M38" s="4">
+      <c r="M38">
         <v>-54.8</v>
       </c>
-      <c r="N38" s="4">
+      <c r="N38">
         <v>-58.2</v>
       </c>
     </row>
     <row r="39" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I39" s="4">
+      <c r="I39">
         <v>-46.3</v>
       </c>
-      <c r="J39" s="4">
+      <c r="J39">
         <v>-38.4</v>
       </c>
       <c r="K39">
         <v>-43.3</v>
       </c>
-      <c r="L39" s="4">
+      <c r="L39">
         <v>-54.9</v>
       </c>
-      <c r="M39" s="4">
+      <c r="M39">
         <v>-54.5</v>
       </c>
-      <c r="N39" s="4">
+      <c r="N39">
         <v>-58.5</v>
       </c>
     </row>
     <row r="40" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I40" s="4">
+      <c r="I40">
         <v>-46.2</v>
       </c>
-      <c r="J40" s="4">
+      <c r="J40">
         <v>-38.799999999999997</v>
       </c>
       <c r="K40">
         <v>-42.8</v>
       </c>
-      <c r="L40" s="4">
+      <c r="L40">
         <v>-55.2</v>
       </c>
-      <c r="M40" s="4">
+      <c r="M40">
         <v>-54.4</v>
       </c>
-      <c r="N40" s="4">
+      <c r="N40">
         <v>-58.3</v>
       </c>
     </row>
     <row r="41" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I41" s="4">
+      <c r="I41">
         <v>-46.2</v>
       </c>
-      <c r="J41" s="4">
+      <c r="J41">
         <v>-39.1</v>
       </c>
       <c r="K41">
         <v>-42.4</v>
       </c>
-      <c r="L41" s="4">
+      <c r="L41">
         <v>-55.5</v>
       </c>
-      <c r="M41" s="4">
+      <c r="M41">
         <v>-54.3</v>
       </c>
-      <c r="N41" s="4">
+      <c r="N41">
         <v>-58</v>
       </c>
-    </row>
-    <row r="42" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I42" s="4"/>
-      <c r="M42" s="4"/>
-      <c r="N42" s="4"/>
-    </row>
-    <row r="43" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I43" s="4"/>
-      <c r="M43" s="4"/>
-      <c r="N43" s="4"/>
-    </row>
-    <row r="44" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I44" s="4"/>
-      <c r="M44" s="4"/>
-      <c r="N44" s="4"/>
-    </row>
-    <row r="45" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I45" s="4"/>
-      <c r="M45" s="4"/>
-      <c r="N45" s="4"/>
-    </row>
-    <row r="46" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I46" s="4"/>
-      <c r="M46" s="4"/>
-      <c r="N46" s="4"/>
-    </row>
-    <row r="47" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-    </row>
-    <row r="48" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I48" s="4"/>
-      <c r="M48" s="4"/>
-      <c r="N48" s="4"/>
-    </row>
-    <row r="49" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I49" s="4"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
-    </row>
-    <row r="50" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="M50" s="4"/>
-      <c r="N50" s="4"/>
-    </row>
-    <row r="51" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="M51" s="4"/>
-      <c r="N51" s="4"/>
-    </row>
-    <row r="52" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="M52" s="4"/>
-      <c r="N52" s="4"/>
-    </row>
-    <row r="53" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="M53" s="4"/>
-      <c r="N53" s="4"/>
-    </row>
-    <row r="54" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="M54" s="4"/>
-    </row>
-    <row r="55" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="M55" s="4"/>
-    </row>
-    <row r="56" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="M56" s="4"/>
-    </row>
-    <row r="57" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="M57" s="4"/>
-    </row>
-    <row r="58" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="M58" s="4"/>
-    </row>
-    <row r="59" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="M59" s="4"/>
-    </row>
-    <row r="60" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="M60" s="4"/>
-    </row>
-    <row r="61" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="M61" s="4"/>
-    </row>
-    <row r="62" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="M62" s="4"/>
-    </row>
-    <row r="63" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="M63" s="4"/>
-    </row>
-    <row r="64" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="M64" s="4"/>
-    </row>
-    <row r="65" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M65" s="4"/>
-    </row>
-    <row r="66" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M66" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added in MAC addresses of other beacons
</commit_message>
<xml_diff>
--- a/Testing RSSI average methods.xlsx
+++ b/Testing RSSI average methods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joryl\Dissertation\dissertation_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69CE79EA-2201-42D9-AB93-529F3FC6891B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D746761A-4D97-4764-BC90-B4AB96ABB558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="6" xr2:uid="{7F11D34D-8D55-4517-9872-D5C4F32D54AF}"/>
   </bookViews>
@@ -2459,7 +2459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{881E5496-3077-4AF9-975C-04A27FA68ED7}">
   <dimension ref="A2:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>

</xml_diff>